<commit_message>
ironed out upload and download in reports page
</commit_message>
<xml_diff>
--- a/host/static/Rate Type.xlsx
+++ b/host/static/Rate Type.xlsx
@@ -372,7 +372,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -387,7 +387,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>

</xml_diff>